<commit_message>
Aanpassingen gedaan om de beslisboom te laten werken met de ministers data. Hier hadden we net andere variabelen voor nodig. Merk op dat voor het gebruik van plot_tree van sklearn versie 0.22 nodig was, terwijl versie 0.19 geinstalleerd was op de omgeving. Ik heb sklearn en numpy hiervoor geupdated.
</commit_message>
<xml_diff>
--- a/Werkboek 1/dataset_wie_is_het_ministers.xlsx
+++ b/Werkboek 1/dataset_wie_is_het_ministers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7640"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -119,12 +119,6 @@
     <t>Bruins</t>
   </si>
   <si>
-    <t>Kleur das</t>
-  </si>
-  <si>
-    <t>Kleur kleding</t>
-  </si>
-  <si>
     <t>Blauw</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Oorbellen</t>
+  </si>
+  <si>
+    <t>Kleur_das</t>
+  </si>
+  <si>
+    <t>Kleur_kleding</t>
   </si>
 </sst>
 </file>
@@ -480,19 +480,19 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -509,22 +509,22 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -541,22 +541,22 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -573,22 +573,22 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -605,22 +605,22 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -637,22 +637,22 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -669,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -678,13 +678,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -701,22 +701,22 @@
         <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -733,22 +733,22 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -765,22 +765,22 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -797,22 +797,22 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,22 +829,22 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -861,22 +861,22 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -893,22 +893,22 @@
         <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -925,22 +925,22 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -957,22 +957,22 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -992,19 +992,19 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1021,22 +1021,22 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>9</v>
@@ -1062,13 +1062,13 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1085,16 +1085,16 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Kleine foutjes in de dataset verbeterd.
</commit_message>
<xml_diff>
--- a/Werkboek 1/dataset_wie_is_het_ministers.xlsx
+++ b/Werkboek 1/dataset_wie_is_het_ministers.xlsx
@@ -86,9 +86,6 @@
     <t>Kaal</t>
   </si>
   <si>
-    <t>Knop</t>
-  </si>
-  <si>
     <t>Ollongren</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Kleur_kleding</t>
+  </si>
+  <si>
+    <t>Knops</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,19 +509,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -541,16 +541,16 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -573,16 +573,16 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -605,16 +605,16 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -637,16 +637,16 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -669,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -701,16 +701,16 @@
         <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -733,16 +733,16 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -765,16 +765,16 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -797,16 +797,16 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
@@ -829,16 +829,16 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -861,16 +861,16 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -893,16 +893,16 @@
         <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -925,16 +925,16 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -957,16 +957,16 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" s="1">
         <v>1</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -992,13 +992,13 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1021,16 +1021,16 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>3</v>
@@ -1053,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>9</v>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
@@ -1085,16 +1085,16 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>

</xml_diff>